<commit_message>
Updated test excel sheet for excelparser
</commit_message>
<xml_diff>
--- a/tests/testonto/excelparser/onto.xlsx
+++ b/tests/testonto/excelparser/onto.xlsx
@@ -1,22 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\francescab\Projects\EMMC\EMMO-python\examples\ontology-from-excel\tool\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\francescab\Projects\EMMC\temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{141FE7E0-D468-40A0-AAA1-3A00B5D427D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B3768AD-8F4A-4168-8D72-5A889E67C260}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="465" yWindow="150" windowWidth="26520" windowHeight="13725" activeTab="1" xr2:uid="{2EA941AB-E9B1-4DC5-9547-722248AB830E}"/>
+    <workbookView xWindow="1335" yWindow="240" windowWidth="35385" windowHeight="22290" activeTab="2" xr2:uid="{2EA941AB-E9B1-4DC5-9547-722248AB830E}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="2" r:id="rId1"/>
-    <sheet name="Concepts" sheetId="1" r:id="rId2"/>
+    <sheet name="ImportedOntologies" sheetId="6" r:id="rId2"/>
+    <sheet name="Concepts" sheetId="1" r:id="rId3"/>
+    <sheet name="ObjectProperties" sheetId="3" r:id="rId4"/>
+    <sheet name="AnnotationProperties" sheetId="4" r:id="rId5"/>
+    <sheet name="DataProperties" sheetId="5" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191028" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="88">
   <si>
     <t>Concept</t>
   </si>
@@ -100,9 +104,6 @@
     <t>Manchester notation, Separate relations with ";"</t>
   </si>
   <si>
-    <t>Data starts on row 4</t>
-  </si>
-  <si>
     <t>Metadata name</t>
   </si>
   <si>
@@ -157,9 +158,6 @@
     <t>Imported ontologies</t>
   </si>
   <si>
-    <t>Full IRI of imported ontologies. Separate with ";"</t>
-  </si>
-  <si>
     <t>Astrid Marthinsen;Georg Schmidt;Jesper Friis;Sylvain Gouttebroze;Tomas Manik;Ulrike Cihak-Bayr</t>
   </si>
   <si>
@@ -244,24 +242,12 @@
     <t>Phase</t>
   </si>
   <si>
-    <t>Particle</t>
-  </si>
-  <si>
-    <t>Precipitate</t>
-  </si>
-  <si>
-    <t>Grain</t>
-  </si>
-  <si>
     <t>hasPart some Boundary</t>
   </si>
   <si>
     <t>Boundary</t>
   </si>
   <si>
-    <t>TemporalBoundary</t>
-  </si>
-  <si>
     <t>SpatialBoundary</t>
   </si>
   <si>
@@ -284,13 +270,46 @@
   </si>
   <si>
     <t>Just;A;Test</t>
+  </si>
+  <si>
+    <t>Object</t>
+  </si>
+  <si>
+    <t>Resolvable URL or path to imported ontologies (one per line )</t>
+  </si>
+  <si>
+    <t>Empty line to test that this does not fail.</t>
+  </si>
+  <si>
+    <t>Data starts on row 4, Test several altLabels</t>
+  </si>
+  <si>
+    <t>Test missing prefLabel (should be completely disregarded)</t>
+  </si>
+  <si>
+    <t>Test prefLabel starting with Number</t>
+  </si>
+  <si>
+    <t>Test PrefLabel containing spaces</t>
+  </si>
+  <si>
+    <t>Test missing parents</t>
+  </si>
+  <si>
+    <t>Test missing elucidation</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Temporal Boundary</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -314,8 +333,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -358,8 +393,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB4C6E7"/>
+        <bgColor rgb="FFB4C7E7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD0CECE"/>
+        <bgColor rgb="FFC9C9C9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -376,11 +423,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -419,6 +475,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -734,9 +794,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEECC088-989A-4277-A366-69DAA3CBC81F}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView zoomScale="292" zoomScaleNormal="292" workbookViewId="0"/>
+    <sheetView zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -747,36 +809,36 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="C1" s="15" t="s">
         <v>23</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C2" s="16"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C3" s="17"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B4">
         <v>0.01</v>
@@ -785,74 +847,66 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C5" s="16"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C6" s="16"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C7" s="16"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="16" t="s">
         <v>31</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="16" t="s">
         <v>33</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B10" s="11"/>
       <c r="C10" s="16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="16" t="s">
         <v>37</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C12" s="16"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13" t="s">
-        <v>81</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>40</v>
-      </c>
+      <c r="C13" s="16"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C14" s="16"/>
@@ -861,7 +915,7 @@
       <c r="C15" s="16"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C16" s="16"/>
+      <c r="C16" s="1"/>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C17" s="1"/>
@@ -874,9 +928,6 @@
     </row>
     <row r="20" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C20" s="1"/>
-    </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C21" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -885,11 +936,44 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E599C59-EBBE-409F-9027-055A4503C4DD}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="120.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68D645D5-E8F4-4C20-A45A-A7B2168B3691}">
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="232" zoomScaleNormal="232" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -923,6 +1007,9 @@
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
       <c r="I1" s="8"/>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
@@ -987,188 +1074,199 @@
     </row>
     <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B4" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H4" s="11"/>
       <c r="J4" s="1" t="s">
-        <v>21</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H5" s="11"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H6" s="11"/>
     </row>
     <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D7" s="11"/>
       <c r="E7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I8" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I10" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C11" s="11"/>
+      <c r="J11" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I12" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G14" t="s">
-        <v>73</v>
+        <v>68</v>
+      </c>
+      <c r="J14" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>57</v>
+        <v>86</v>
       </c>
       <c r="G15" t="s">
-        <v>73</v>
+        <v>68</v>
+      </c>
+      <c r="J15" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G20" t="s">
-        <v>78</v>
+        <v>66</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="J16" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G17" t="s">
+        <v>72</v>
+      </c>
+      <c r="J17" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="J18" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1181,13 +1279,112 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41DA0DD4-0FE3-4697-86E8-79E6CA6FFC1A}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C40FDD2F-AB3E-416A-B879-D38E3CF3242F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C22304DB-D820-4C49-876B-6DD7EE7426E1}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J49" sqref="J49"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <CorpSiteZipContact xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteProjectLeader xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </CorpSiteProjectLeader>
+    <CorpSiteSubTitle xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteTags xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteISBN xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpWorkflowFeedback xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteAccess xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">Kun navngitte medlemmer</CorpSiteAccess>
+    <CorpSiteRecipientPerson xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteProjectNumber xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteProjectName xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpDocInstitute xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteInstitutePhone xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpWorkflowStatus xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteProjectOwner xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </CorpSiteProjectOwner>
+    <CorpDocPageClassificationNbNo xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">Åpen</CorpDocPageClassificationNbNo>
+    <CorpDocClassificationEnUs xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">Unrestricted</CorpDocClassificationEnUs>
+    <CorpDocClassificationNbNo xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">Åpen</CorpDocClassificationNbNo>
+    <CorpSiteClassification xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">Åpen</CorpSiteClassification>
+    <CorpSiteInstituteEmail xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteCoAuthors xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteDocumentAuthor xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </CorpSiteDocumentAuthor>
+    <CorpSiteInstituteEnUs xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteRecipientCompany xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteDocLanguage xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpDocVersion xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpWorkflowApproval xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <ArchiveStatus xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteProjectQA xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </CorpSiteProjectQA>
+    <CorpSiteZipAddress xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteVATNumber xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteReportNumber xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteOurRef xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpDocPageClassificationEnUs xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">Unrestricted</CorpDocPageClassificationEnUs>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1710,73 +1907,28 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <CorpSiteZipContact xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteProjectLeader xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </CorpSiteProjectLeader>
-    <CorpSiteSubTitle xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteTags xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteISBN xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpWorkflowFeedback xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteAccess xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">Kun navngitte medlemmer</CorpSiteAccess>
-    <CorpSiteRecipientPerson xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteProjectNumber xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteProjectName xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpDocInstitute xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteInstitutePhone xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpWorkflowStatus xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteProjectOwner xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </CorpSiteProjectOwner>
-    <CorpDocPageClassificationNbNo xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">Åpen</CorpDocPageClassificationNbNo>
-    <CorpDocClassificationEnUs xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">Unrestricted</CorpDocClassificationEnUs>
-    <CorpDocClassificationNbNo xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">Åpen</CorpDocClassificationNbNo>
-    <CorpSiteClassification xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">Åpen</CorpSiteClassification>
-    <CorpSiteInstituteEmail xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteCoAuthors xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteDocumentAuthor xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </CorpSiteDocumentAuthor>
-    <CorpSiteInstituteEnUs xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteRecipientCompany xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteDocLanguage xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpDocVersion xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpWorkflowApproval xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <ArchiveStatus xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteProjectQA xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </CorpSiteProjectQA>
-    <CorpSiteZipAddress xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteVATNumber xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteReportNumber xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteOurRef xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpDocPageClassificationEnUs xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">Unrestricted</CorpDocPageClassificationEnUs>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C5504F3-8457-4CD0-9BA4-F4E5EEC4ABF3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95E916DF-5697-4D04-9AE8-BCDE5705DE19}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="f0e54009-8c9c-44b5-8b9b-dd795f6c992f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="8bbd4995-53b7-43e2-b62f-10947586ac31"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="c4cb6b28-ce9b-4437-9d9c-1e653dd193be"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1802,19 +1954,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95E916DF-5697-4D04-9AE8-BCDE5705DE19}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C5504F3-8457-4CD0-9BA4-F4E5EEC4ABF3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="f0e54009-8c9c-44b5-8b9b-dd795f6c992f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="8bbd4995-53b7-43e2-b62f-10947586ac31"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="c4cb6b28-ce9b-4437-9d9c-1e653dd193be"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Excelparser now proceeds if force is true, diregarding concepts that cannot be added due to errors in prefLabel: prefLabels with spaces, concepts that already exist (These are diregarded - it might be good to add an option for these in the future if it should be allowed to change or add to concepts), concepts where prefLabel is completely missing. Concepts missing elucidation OK. Leading and trailing spaces are removed.
</commit_message>
<xml_diff>
--- a/tests/testonto/excelparser/onto.xlsx
+++ b/tests/testonto/excelparser/onto.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\francescab\Projects\EMMC\temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B3768AD-8F4A-4168-8D72-5A889E67C260}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EEB799F-350C-4A87-B6B5-EA12A7C7B18D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1335" yWindow="240" windowWidth="35385" windowHeight="22290" activeTab="2" xr2:uid="{2EA941AB-E9B1-4DC5-9547-722248AB830E}"/>
+    <workbookView xWindow="12015" yWindow="2325" windowWidth="24750" windowHeight="20430" activeTab="2" xr2:uid="{2EA941AB-E9B1-4DC5-9547-722248AB830E}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="97">
   <si>
     <t>Concept</t>
   </si>
@@ -158,12 +158,6 @@
     <t>Imported ontologies</t>
   </si>
   <si>
-    <t>Astrid Marthinsen;Georg Schmidt;Jesper Friis;Sylvain Gouttebroze;Tomas Manik;Ulrike Cihak-Bayr</t>
-  </si>
-  <si>
-    <t>Microstructure ontology based on EMMO - Top concepts</t>
-  </si>
-  <si>
     <t>Pattern</t>
   </si>
   <si>
@@ -239,9 +233,6 @@
     <t>SpatialPattern;FinitePattern</t>
   </si>
   <si>
-    <t>Phase</t>
-  </si>
-  <si>
     <t>hasPart some Boundary</t>
   </si>
   <si>
@@ -281,15 +272,9 @@
     <t>Empty line to test that this does not fail.</t>
   </si>
   <si>
-    <t>Data starts on row 4, Test several altLabels</t>
-  </si>
-  <si>
     <t>Test missing prefLabel (should be completely disregarded)</t>
   </si>
   <si>
-    <t>Test prefLabel starting with Number</t>
-  </si>
-  <si>
     <t>Test PrefLabel containing spaces</t>
   </si>
   <si>
@@ -303,6 +288,48 @@
   </si>
   <si>
     <t>Temporal Boundary</t>
+  </si>
+  <si>
+    <t>Test several altLabels</t>
+  </si>
+  <si>
+    <t>Data starts on row 4, Test parent from imrted ontology</t>
+  </si>
+  <si>
+    <t>Test prefLabel is only spaces</t>
+  </si>
+  <si>
+    <t>Test adding concept that already exists (in and imported ontology)</t>
+  </si>
+  <si>
+    <t>Jesper Friis;Sylvain Gouttebroze;Francesca L. Bleken</t>
+  </si>
+  <si>
+    <t>A test domain ontology</t>
+  </si>
+  <si>
+    <t>SINTEF;SINTEF Industry</t>
+  </si>
+  <si>
+    <t>Test several relations</t>
+  </si>
+  <si>
+    <t>Test several parents</t>
+  </si>
+  <si>
+    <t>Test prefLabel with leading or trailing spaces</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Boundary </t>
+  </si>
+  <si>
+    <t>Test prefLabel starting with Number, this is currently allowed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        </t>
+  </si>
+  <si>
+    <t>Atom</t>
   </si>
 </sst>
 </file>
@@ -473,12 +500,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -797,7 +824,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -823,7 +850,7 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C2" s="16"/>
     </row>
@@ -832,7 +859,7 @@
         <v>25</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C3" s="17"/>
     </row>
@@ -850,7 +877,7 @@
         <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>88</v>
       </c>
       <c r="C5" s="16"/>
     </row>
@@ -879,7 +906,7 @@
         <v>32</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>39</v>
+        <v>87</v>
       </c>
       <c r="C9" s="16" t="s">
         <v>33</v>
@@ -889,7 +916,9 @@
       <c r="A10" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="11"/>
+      <c r="B10" s="11" t="s">
+        <v>89</v>
+      </c>
       <c r="C10" s="16" t="s">
         <v>35</v>
       </c>
@@ -949,18 +978,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
-        <v>78</v>
+      <c r="A2" s="19" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -970,10 +999,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68D645D5-E8F4-4C20-A45A-A7B2168B3691}">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -994,16 +1023,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18" t="s">
+      <c r="B1" s="20"/>
+      <c r="C1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
       <c r="I1" s="8"/>
@@ -1074,199 +1103,227 @@
     </row>
     <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B4" t="s">
-        <v>76</v>
+        <v>39</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H4" s="11"/>
       <c r="J4" s="1" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>40</v>
+      </c>
+      <c r="B5" t="s">
+        <v>73</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H5" s="11"/>
+      <c r="J5" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H6" s="11"/>
     </row>
     <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D7" s="11"/>
       <c r="E7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I8" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G9" t="s">
-        <v>63</v>
+        <v>61</v>
+      </c>
+      <c r="J9" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I10" t="s">
-        <v>71</v>
+        <v>68</v>
+      </c>
+      <c r="J10" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C11" s="11"/>
       <c r="J11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I12" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>68</v>
+        <v>93</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G13" t="s">
-        <v>62</v>
+        <v>60</v>
+      </c>
+      <c r="J13" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G14" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J14" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="G15" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J15" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>66</v>
-      </c>
       <c r="C16" s="11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J16" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G17" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="J17" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1</v>
       </c>
+      <c r="G18" t="s">
+        <v>69</v>
+      </c>
       <c r="J18" t="s">
-        <v>82</v>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>95</v>
+      </c>
+      <c r="J19" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>96</v>
+      </c>
+      <c r="J20" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1289,7 +1346,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1324,70 +1381,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <CorpSiteZipContact xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteProjectLeader xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </CorpSiteProjectLeader>
-    <CorpSiteSubTitle xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteTags xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteISBN xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpWorkflowFeedback xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteAccess xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">Kun navngitte medlemmer</CorpSiteAccess>
-    <CorpSiteRecipientPerson xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteProjectNumber xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteProjectName xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpDocInstitute xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteInstitutePhone xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpWorkflowStatus xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteProjectOwner xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </CorpSiteProjectOwner>
-    <CorpDocPageClassificationNbNo xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">Åpen</CorpDocPageClassificationNbNo>
-    <CorpDocClassificationEnUs xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">Unrestricted</CorpDocClassificationEnUs>
-    <CorpDocClassificationNbNo xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">Åpen</CorpDocClassificationNbNo>
-    <CorpSiteClassification xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">Åpen</CorpSiteClassification>
-    <CorpSiteInstituteEmail xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteCoAuthors xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteDocumentAuthor xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </CorpSiteDocumentAuthor>
-    <CorpSiteInstituteEnUs xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteRecipientCompany xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteDocLanguage xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpDocVersion xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpWorkflowApproval xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <ArchiveStatus xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteProjectQA xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </CorpSiteProjectQA>
-    <CorpSiteZipAddress xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteVATNumber xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteReportNumber xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteOurRef xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpDocPageClassificationEnUs xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">Unrestricted</CorpDocPageClassificationEnUs>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Generic document" ma:contentTypeID="0x01010031B82B69D2361148B4D8F7EC156802130800135FF0806A5B6E4A82730A8DA96F38E4" ma:contentTypeVersion="42" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cf3ec053e01706e36cc905dbd1cf3891">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8bbd4995-53b7-43e2-b62f-10947586ac31" xmlns:ns3="f0e54009-8c9c-44b5-8b9b-dd795f6c992f" xmlns:ns4="c4cb6b28-ce9b-4437-9d9c-1e653dd193be" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cc4cb9f9d9eaebfce8e7fc49d63413d7" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="8bbd4995-53b7-43e2-b62f-10947586ac31"/>
@@ -1906,6 +1899,70 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <CorpSiteZipContact xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteProjectLeader xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </CorpSiteProjectLeader>
+    <CorpSiteSubTitle xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteTags xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteISBN xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpWorkflowFeedback xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteAccess xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">Kun navngitte medlemmer</CorpSiteAccess>
+    <CorpSiteRecipientPerson xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteProjectNumber xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteProjectName xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpDocInstitute xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteInstitutePhone xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpWorkflowStatus xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteProjectOwner xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </CorpSiteProjectOwner>
+    <CorpDocPageClassificationNbNo xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">Åpen</CorpDocPageClassificationNbNo>
+    <CorpDocClassificationEnUs xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">Unrestricted</CorpDocClassificationEnUs>
+    <CorpDocClassificationNbNo xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">Åpen</CorpDocClassificationNbNo>
+    <CorpSiteClassification xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">Åpen</CorpSiteClassification>
+    <CorpSiteInstituteEmail xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteCoAuthors xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteDocumentAuthor xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </CorpSiteDocumentAuthor>
+    <CorpSiteInstituteEnUs xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteRecipientCompany xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteDocLanguage xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpDocVersion xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpWorkflowApproval xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <ArchiveStatus xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteProjectQA xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </CorpSiteProjectQA>
+    <CorpSiteZipAddress xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteVATNumber xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteReportNumber xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteOurRef xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpDocPageClassificationEnUs xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">Unrestricted</CorpDocPageClassificationEnUs>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1916,24 +1973,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95E916DF-5697-4D04-9AE8-BCDE5705DE19}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="f0e54009-8c9c-44b5-8b9b-dd795f6c992f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="8bbd4995-53b7-43e2-b62f-10947586ac31"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="c4cb6b28-ce9b-4437-9d9c-1e653dd193be"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06A8E286-8EB5-40D3-9A71-29AF5D9413D2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1953,6 +1992,24 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95E916DF-5697-4D04-9AE8-BCDE5705DE19}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="f0e54009-8c9c-44b5-8b9b-dd795f6c992f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="8bbd4995-53b7-43e2-b62f-10947586ac31"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="c4cb6b28-ce9b-4437-9d9c-1e653dd193be"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C5504F3-8457-4CD0-9BA4-F4E5EEC4ABF3}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
If missing or wrong parents, concepts are defined directly under owlready2.Thing
</commit_message>
<xml_diff>
--- a/tests/testonto/excelparser/onto.xlsx
+++ b/tests/testonto/excelparser/onto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\francescab\Projects\EMMC\temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EEB799F-350C-4A87-B6B5-EA12A7C7B18D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD7E2C29-86BA-4859-9C20-218617D0C07D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12015" yWindow="2325" windowWidth="24750" windowHeight="20430" activeTab="2" xr2:uid="{2EA941AB-E9B1-4DC5-9547-722248AB830E}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="98">
   <si>
     <t>Concept</t>
   </si>
@@ -293,9 +293,6 @@
     <t>Test several altLabels</t>
   </si>
   <si>
-    <t>Data starts on row 4, Test parent from imrted ontology</t>
-  </si>
-  <si>
     <t>Test prefLabel is only spaces</t>
   </si>
   <si>
@@ -330,6 +327,12 @@
   </si>
   <si>
     <t>Atom</t>
+  </si>
+  <si>
+    <t>SpatioTemporalBoundary</t>
+  </si>
+  <si>
+    <t>Data starts on row 4, Test parent from imported ontology</t>
   </si>
 </sst>
 </file>
@@ -877,7 +880,7 @@
         <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C5" s="16"/>
     </row>
@@ -906,7 +909,7 @@
         <v>32</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C9" s="16" t="s">
         <v>33</v>
@@ -917,7 +920,7 @@
         <v>34</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C10" s="16" t="s">
         <v>35</v>
@@ -1001,8 +1004,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68D645D5-E8F4-4C20-A45A-A7B2168B3691}">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1116,7 +1119,7 @@
       </c>
       <c r="H4" s="11"/>
       <c r="J4" s="1" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1195,7 +1198,7 @@
         <v>61</v>
       </c>
       <c r="J9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -1215,7 +1218,7 @@
         <v>68</v>
       </c>
       <c r="J10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -1243,7 +1246,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C13" s="11" t="s">
         <v>53</v>
@@ -1252,7 +1255,7 @@
         <v>60</v>
       </c>
       <c r="J13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1284,6 +1287,9 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>96</v>
+      </c>
       <c r="C16" s="11" t="s">
         <v>53</v>
       </c>
@@ -1307,23 +1313,23 @@
         <v>69</v>
       </c>
       <c r="J18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Work in progress: fixing not-yet-defined-parent
</commit_message>
<xml_diff>
--- a/tests/testonto/excelparser/onto.xlsx
+++ b/tests/testonto/excelparser/onto.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="105">
   <si>
     <t xml:space="preserve">Metadata name</t>
   </si>
@@ -168,13 +168,25 @@
     <t xml:space="preserve">GrainBoundary</t>
   </si>
   <si>
-    <t xml:space="preserve">The boundary of a Grain</t>
+    <t xml:space="preserve">The boundary of a grain</t>
   </si>
   <si>
     <t xml:space="preserve">SpatialBoundary</t>
   </si>
   <si>
-    <t xml:space="preserve">Test parent defined later</t>
+    <t xml:space="preserve">Test not-yet-defined parent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SubgrainBoundary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The boundary of a subgrain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LowAngleGrainBoundary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test of undefined parent</t>
   </si>
   <si>
     <t xml:space="preserve">Pattern</t>
@@ -811,10 +823,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="96" zoomScaleNormal="96" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J4" activeCellId="0" sqref="J4"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -927,39 +939,35 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="G5" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="G5" s="0" t="s">
+      <c r="J5" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="H5" s="8"/>
-      <c r="J5" s="9" t="s">
+    </row>
+    <row r="6" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="C6" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="D6" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="G6" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="G6" s="0" t="s">
-        <v>50</v>
-      </c>
       <c r="H6" s="8"/>
-      <c r="J6" s="0" t="s">
+      <c r="J6" s="9" t="s">
         <v>58</v>
       </c>
     </row>
@@ -967,192 +975,210 @@
       <c r="A7" s="0" t="s">
         <v>59</v>
       </c>
+      <c r="B7" s="0" t="s">
+        <v>60</v>
+      </c>
       <c r="C7" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="E7" s="0" t="s">
         <v>61</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H7" s="8"/>
-    </row>
-    <row r="8" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J7" s="0" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="D8" s="8"/>
+        <v>64</v>
+      </c>
       <c r="E8" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>55</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="H8" s="8"/>
     </row>
     <row r="9" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="D9" s="0" t="s">
         <v>67</v>
       </c>
+      <c r="D9" s="8"/>
+      <c r="E9" s="0" t="s">
+        <v>68</v>
+      </c>
       <c r="G9" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="I9" s="0" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>69</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>57</v>
+        <v>70</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>71</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="J10" s="0" t="s">
-        <v>71</v>
+        <v>54</v>
+      </c>
+      <c r="I10" s="0" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="E11" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="G11" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="G11" s="0" t="s">
+      <c r="J11" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="I11" s="0" t="s">
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="J11" s="0" t="s">
+      <c r="C12" s="8" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="8"/>
+      <c r="E12" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="I12" s="0" t="s">
+        <v>80</v>
+      </c>
       <c r="J12" s="0" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="E13" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="G13" s="0" t="s">
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C13" s="8"/>
+      <c r="J13" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="I13" s="0" t="s">
+    </row>
+    <row r="14" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="C14" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="C14" s="8" t="s">
-        <v>57</v>
+      <c r="E14" s="0" t="s">
+        <v>85</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="J14" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
+      </c>
+      <c r="I14" s="0" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C15" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="G15" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="G15" s="0" t="s">
-        <v>87</v>
-      </c>
       <c r="J15" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>48</v>
+        <v>90</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>89</v>
+        <v>61</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="G17" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="C17" s="8" t="s">
-        <v>57</v>
-      </c>
       <c r="J17" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G18" s="0" t="s">
-        <v>93</v>
+      <c r="A18" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>61</v>
       </c>
       <c r="J18" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="n">
+      <c r="G19" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="J19" s="0" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="G19" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="J19" s="0" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>96</v>
+      <c r="G20" s="0" t="s">
+        <v>97</v>
       </c>
       <c r="J20" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="J21" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="J22" s="0" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1185,7 +1211,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added test to check that all concpets thata are defined in the pwrong manner are listed in the error dictionary returned
</commit_message>
<xml_diff>
--- a/tests/testonto/excelparser/onto.xlsx
+++ b/tests/testonto/excelparser/onto.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\francescab\Projects\EMMC\temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\francescab\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9862AFBE-285D-4D03-87FE-3024212D0041}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF9571AF-EC9A-4CD9-9D4D-B1EF2C83D15E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="34500" windowHeight="20430" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="38700" windowHeight="15435" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="110">
   <si>
     <t>Metadata name</t>
   </si>
@@ -341,9 +341,6 @@
     <t>Atom</t>
   </si>
   <si>
-    <t>Test adding concept that already exists (in and imported ontology)</t>
-  </si>
-  <si>
     <t>Object</t>
   </si>
   <si>
@@ -357,6 +354,12 @@
   </si>
   <si>
     <t>Test invalid parent</t>
+  </si>
+  <si>
+    <t>Test adding concept that already exists in and imported ontology)</t>
+  </si>
+  <si>
+    <t>Test defining same concept twice in the same excel sheet</t>
   </si>
 </sst>
 </file>
@@ -455,9 +458,6 @@
   </cellStyleXfs>
   <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -493,6 +493,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -889,91 +892,91 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="4"/>
+      <c r="C2" s="3"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="7"/>
+      <c r="C3" s="6"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B4">
         <v>0.01</v>
       </c>
-      <c r="C4" s="4"/>
+      <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="4"/>
+      <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="4"/>
+      <c r="C6" s="3"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="4"/>
+      <c r="C7" s="3"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>19</v>
       </c>
     </row>
@@ -981,36 +984,36 @@
       <c r="A11" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C12" s="4"/>
+      <c r="C12" s="3"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C13" s="4"/>
+      <c r="C13" s="3"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C14" s="4"/>
+      <c r="C14" s="3"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C15" s="4"/>
+      <c r="C15" s="3"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C16" s="10"/>
+      <c r="C16" s="9"/>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C17" s="10"/>
+      <c r="C17" s="9"/>
     </row>
     <row r="18" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C18" s="10"/>
+      <c r="C18" s="9"/>
     </row>
     <row r="19" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C19" s="10"/>
+      <c r="C19" s="9"/>
     </row>
     <row r="20" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C20" s="10"/>
+      <c r="C20" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -1032,12 +1035,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1054,10 +1057,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1078,81 +1081,81 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="18"/>
+      <c r="C1" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="13"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="12"/>
       <c r="J1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="H2" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="I2" s="17" t="s">
+      <c r="I2" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="J2" s="9" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="I3" s="18" t="s">
+      <c r="I3" s="17" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1186,30 +1189,30 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G6" t="s">
         <v>52</v>
       </c>
       <c r="J6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>54</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="8" t="s">
         <v>56</v>
       </c>
       <c r="G7" t="s">
         <v>57</v>
       </c>
-      <c r="H7" s="9"/>
-      <c r="J7" s="10" t="s">
+      <c r="H7" s="8"/>
+      <c r="J7" s="9" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1220,13 +1223,13 @@
       <c r="B8" t="s">
         <v>60</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="8" t="s">
         <v>61</v>
       </c>
       <c r="G8" t="s">
         <v>54</v>
       </c>
-      <c r="H8" s="9"/>
+      <c r="H8" s="8"/>
       <c r="J8" t="s">
         <v>62</v>
       </c>
@@ -1235,28 +1238,28 @@
       <c r="A9" t="s">
         <v>63</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="8" t="s">
         <v>64</v>
       </c>
       <c r="E9" t="s">
         <v>65</v>
       </c>
       <c r="G9" t="s">
+        <v>106</v>
+      </c>
+      <c r="H9" s="8"/>
+      <c r="J9" t="s">
         <v>107</v>
-      </c>
-      <c r="H9" s="9"/>
-      <c r="J9" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>66</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="D10" s="9"/>
+      <c r="D10" s="8"/>
       <c r="E10" t="s">
         <v>68</v>
       </c>
@@ -1268,7 +1271,7 @@
       <c r="A11" t="s">
         <v>69</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="8" t="s">
         <v>70</v>
       </c>
       <c r="D11" t="s">
@@ -1285,7 +1288,7 @@
       <c r="A12" t="s">
         <v>73</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="8" t="s">
         <v>61</v>
       </c>
       <c r="G12" t="s">
@@ -1299,7 +1302,7 @@
       <c r="A13" t="s">
         <v>76</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="8" t="s">
         <v>77</v>
       </c>
       <c r="E13" t="s">
@@ -1316,7 +1319,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C14" s="9"/>
+      <c r="C14" s="8"/>
       <c r="J14" t="s">
         <v>82</v>
       </c>
@@ -1325,7 +1328,7 @@
       <c r="A15" t="s">
         <v>83</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="8" t="s">
         <v>84</v>
       </c>
       <c r="E15" t="s">
@@ -1342,7 +1345,7 @@
       <c r="A16" t="s">
         <v>88</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="8" t="s">
         <v>61</v>
       </c>
       <c r="G16" t="s">
@@ -1356,7 +1359,7 @@
       <c r="A17" t="s">
         <v>90</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="8" t="s">
         <v>61</v>
       </c>
       <c r="G17" t="s">
@@ -1370,7 +1373,7 @@
       <c r="A18" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="8" t="s">
         <v>93</v>
       </c>
       <c r="G18" t="s">
@@ -1384,7 +1387,7 @@
       <c r="A19" t="s">
         <v>95</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="8" t="s">
         <v>61</v>
       </c>
       <c r="J19" t="s">
@@ -1423,7 +1426,23 @@
         <v>102</v>
       </c>
       <c r="J23" t="s">
-        <v>103</v>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D24" s="8"/>
+      <c r="G24" t="s">
+        <v>57</v>
+      </c>
+      <c r="H24" s="8"/>
+      <c r="J24" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1446,7 +1465,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
create_from_excel/pandas return as list of concepts that are worngly defined in the excelfile (#396)
* Added returning errors in excelparser

* Added test to check that all concpets that are defined in the wrong manner are listed in the error dictionary returned.

* Documented new output from excelparser
</commit_message>
<xml_diff>
--- a/tests/testonto/excelparser/onto.xlsx
+++ b/tests/testonto/excelparser/onto.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\francescab\Projects\EMMC\temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\francescab\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9862AFBE-285D-4D03-87FE-3024212D0041}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF9571AF-EC9A-4CD9-9D4D-B1EF2C83D15E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="34500" windowHeight="20430" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="38700" windowHeight="15435" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="110">
   <si>
     <t>Metadata name</t>
   </si>
@@ -341,9 +341,6 @@
     <t>Atom</t>
   </si>
   <si>
-    <t>Test adding concept that already exists (in and imported ontology)</t>
-  </si>
-  <si>
     <t>Object</t>
   </si>
   <si>
@@ -357,6 +354,12 @@
   </si>
   <si>
     <t>Test invalid parent</t>
+  </si>
+  <si>
+    <t>Test adding concept that already exists in and imported ontology)</t>
+  </si>
+  <si>
+    <t>Test defining same concept twice in the same excel sheet</t>
   </si>
 </sst>
 </file>
@@ -455,9 +458,6 @@
   </cellStyleXfs>
   <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -493,6 +493,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -889,91 +892,91 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="4"/>
+      <c r="C2" s="3"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="7"/>
+      <c r="C3" s="6"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B4">
         <v>0.01</v>
       </c>
-      <c r="C4" s="4"/>
+      <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="4"/>
+      <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="4"/>
+      <c r="C6" s="3"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="4"/>
+      <c r="C7" s="3"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>19</v>
       </c>
     </row>
@@ -981,36 +984,36 @@
       <c r="A11" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C12" s="4"/>
+      <c r="C12" s="3"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C13" s="4"/>
+      <c r="C13" s="3"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C14" s="4"/>
+      <c r="C14" s="3"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C15" s="4"/>
+      <c r="C15" s="3"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C16" s="10"/>
+      <c r="C16" s="9"/>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C17" s="10"/>
+      <c r="C17" s="9"/>
     </row>
     <row r="18" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C18" s="10"/>
+      <c r="C18" s="9"/>
     </row>
     <row r="19" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C19" s="10"/>
+      <c r="C19" s="9"/>
     </row>
     <row r="20" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C20" s="10"/>
+      <c r="C20" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -1032,12 +1035,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1054,10 +1057,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1078,81 +1081,81 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="18"/>
+      <c r="C1" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="13"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="12"/>
       <c r="J1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="H2" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="I2" s="17" t="s">
+      <c r="I2" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="J2" s="9" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="I3" s="18" t="s">
+      <c r="I3" s="17" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1186,30 +1189,30 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G6" t="s">
         <v>52</v>
       </c>
       <c r="J6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>54</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="8" t="s">
         <v>56</v>
       </c>
       <c r="G7" t="s">
         <v>57</v>
       </c>
-      <c r="H7" s="9"/>
-      <c r="J7" s="10" t="s">
+      <c r="H7" s="8"/>
+      <c r="J7" s="9" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1220,13 +1223,13 @@
       <c r="B8" t="s">
         <v>60</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="8" t="s">
         <v>61</v>
       </c>
       <c r="G8" t="s">
         <v>54</v>
       </c>
-      <c r="H8" s="9"/>
+      <c r="H8" s="8"/>
       <c r="J8" t="s">
         <v>62</v>
       </c>
@@ -1235,28 +1238,28 @@
       <c r="A9" t="s">
         <v>63</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="8" t="s">
         <v>64</v>
       </c>
       <c r="E9" t="s">
         <v>65</v>
       </c>
       <c r="G9" t="s">
+        <v>106</v>
+      </c>
+      <c r="H9" s="8"/>
+      <c r="J9" t="s">
         <v>107</v>
-      </c>
-      <c r="H9" s="9"/>
-      <c r="J9" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>66</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="D10" s="9"/>
+      <c r="D10" s="8"/>
       <c r="E10" t="s">
         <v>68</v>
       </c>
@@ -1268,7 +1271,7 @@
       <c r="A11" t="s">
         <v>69</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="8" t="s">
         <v>70</v>
       </c>
       <c r="D11" t="s">
@@ -1285,7 +1288,7 @@
       <c r="A12" t="s">
         <v>73</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="8" t="s">
         <v>61</v>
       </c>
       <c r="G12" t="s">
@@ -1299,7 +1302,7 @@
       <c r="A13" t="s">
         <v>76</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="8" t="s">
         <v>77</v>
       </c>
       <c r="E13" t="s">
@@ -1316,7 +1319,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C14" s="9"/>
+      <c r="C14" s="8"/>
       <c r="J14" t="s">
         <v>82</v>
       </c>
@@ -1325,7 +1328,7 @@
       <c r="A15" t="s">
         <v>83</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="8" t="s">
         <v>84</v>
       </c>
       <c r="E15" t="s">
@@ -1342,7 +1345,7 @@
       <c r="A16" t="s">
         <v>88</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="8" t="s">
         <v>61</v>
       </c>
       <c r="G16" t="s">
@@ -1356,7 +1359,7 @@
       <c r="A17" t="s">
         <v>90</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="8" t="s">
         <v>61</v>
       </c>
       <c r="G17" t="s">
@@ -1370,7 +1373,7 @@
       <c r="A18" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="8" t="s">
         <v>93</v>
       </c>
       <c r="G18" t="s">
@@ -1384,7 +1387,7 @@
       <c r="A19" t="s">
         <v>95</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="8" t="s">
         <v>61</v>
       </c>
       <c r="J19" t="s">
@@ -1423,7 +1426,23 @@
         <v>102</v>
       </c>
       <c r="J23" t="s">
-        <v>103</v>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D24" s="8"/>
+      <c r="G24" t="s">
+        <v>57</v>
+      </c>
+      <c r="H24" s="8"/>
+      <c r="J24" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1446,7 +1465,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Allow for adding prefix in manchester notation. (#469)
it is now possible to use e.g. 'emmo:hasPart some emmo:Atom" in the string to be evaluated as manchester notation. A test was added for this in test_manchester.py and examples were added to the onto.xlsx used in the excelparser for testing.
</commit_message>
<xml_diff>
--- a/tests/testonto/excelparser/onto.xlsx
+++ b/tests/testonto/excelparser/onto.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\francescab\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sintef-my.sharepoint.com/personal/francesca_l_bleken_sintef_no/Documents/Skrivebord/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF9571AF-EC9A-4CD9-9D4D-B1EF2C83D15E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="66" documentId="13_ncr:1_{BF9571AF-EC9A-4CD9-9D4D-B1EF2C83D15E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{32CC4B7C-17CE-438B-BDCB-AE6F9A899A12}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="38700" windowHeight="15435" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="52380" yWindow="-1785" windowWidth="34740" windowHeight="17895" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="125">
   <si>
     <t>Metadata name</t>
   </si>
@@ -360,13 +360,58 @@
   </si>
   <si>
     <t>Test defining same concept twice in the same excel sheet</t>
+  </si>
+  <si>
+    <t>SpecialMolecule</t>
+  </si>
+  <si>
+    <t>Our own special molecules</t>
+  </si>
+  <si>
+    <t>Used for our own special purpose</t>
+  </si>
+  <si>
+    <t>hasPart some Atom</t>
+  </si>
+  <si>
+    <t>prefix</t>
+  </si>
+  <si>
+    <t>emmo</t>
+  </si>
+  <si>
+    <t>AnotherSpecialMolecule</t>
+  </si>
+  <si>
+    <t>Molecule</t>
+  </si>
+  <si>
+    <t>emmo-inferred-chemistry2:Molecule</t>
+  </si>
+  <si>
+    <t>emmo-inferred-chemistry2:hasPart  some emmo-inferred-chemistry2:Atom</t>
+  </si>
+  <si>
+    <t>Test giving prefix from emmo for subclass of and relations. Will be changed to emmo: when prefix is fixed</t>
+  </si>
+  <si>
+    <t>Test giving prefix to relations. Will be changed to emmo: when prefix is fixed</t>
+  </si>
+  <si>
+    <t>base_iri_root</t>
+  </si>
+  <si>
+    <t>If base_iri_root is given, all imported ontologies whose base_iri starts with base_iri_root will be given the same prefix.</t>
+  </si>
+  <si>
+    <t>Local prefix for the imported ontology.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -386,6 +431,14 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -453,10 +506,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -493,11 +547,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperkobling" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -582,7 +638,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -884,7 +940,7 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.42578125" customWidth="1"/>
     <col min="2" max="2" width="120.140625" customWidth="1"/>
@@ -1023,47 +1079,75 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="120.140625" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" customWidth="1"/>
+    <col min="3" max="3" width="28.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B2" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
         <v>24</v>
       </c>
+      <c r="B3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C4" s="18"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>93</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{4AE6D9F9-5AA3-467D-A245-2C36C0027930}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+    <sheetView topLeftCell="C1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.28515625" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
@@ -1073,7 +1157,7 @@
     <col min="6" max="6" width="19.140625" customWidth="1"/>
     <col min="7" max="7" width="33.42578125" customWidth="1"/>
     <col min="8" max="8" width="18.28515625" customWidth="1"/>
-    <col min="9" max="9" width="45.85546875" customWidth="1"/>
+    <col min="9" max="9" width="69.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
     <col min="11" max="11" width="12.85546875" customWidth="1"/>
     <col min="12" max="12" width="14.85546875" customWidth="1"/>
@@ -1081,16 +1165,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18" t="s">
+      <c r="B1" s="19"/>
+      <c r="C1" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
       <c r="G1" s="11"/>
       <c r="H1" s="11"/>
       <c r="I1" s="12"/>
@@ -1324,7 +1408,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>83</v>
       </c>
@@ -1443,6 +1527,40 @@
       <c r="H24" s="8"/>
       <c r="J24" t="s">
         <v>109</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>110</v>
+      </c>
+      <c r="C25" t="s">
+        <v>111</v>
+      </c>
+      <c r="D25" t="s">
+        <v>112</v>
+      </c>
+      <c r="G25" t="s">
+        <v>118</v>
+      </c>
+      <c r="I25" t="s">
+        <v>113</v>
+      </c>
+      <c r="J25" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>116</v>
+      </c>
+      <c r="G26" t="s">
+        <v>117</v>
+      </c>
+      <c r="I26" t="s">
+        <v>119</v>
+      </c>
+      <c r="J26" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -1461,7 +1579,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1480,7 +1598,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -1495,7 +1613,7 @@
       <selection activeCell="J49" sqref="J49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Setting prefix explicitly in excelparser
Prefix can now be set explicitly for imported ontologies in excelparser.
Either only prefix of given ontology, or set common prefix for all
ontologies with a given root in the base_iri
</commit_message>
<xml_diff>
--- a/tests/testonto/excelparser/onto.xlsx
+++ b/tests/testonto/excelparser/onto.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sintef-my.sharepoint.com/personal/francesca_l_bleken_sintef_no/Documents/Skrivebord/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="66" documentId="13_ncr:1_{BF9571AF-EC9A-4CD9-9D4D-B1EF2C83D15E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{32CC4B7C-17CE-438B-BDCB-AE6F9A899A12}"/>
+  <xr:revisionPtr revIDLastSave="92" documentId="13_ncr:1_{BF9571AF-EC9A-4CD9-9D4D-B1EF2C83D15E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7C4AA229-0711-4128-97D8-805D85E67D3B}"/>
   <bookViews>
-    <workbookView xWindow="52380" yWindow="-1785" windowWidth="34740" windowHeight="17895" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="37230" windowHeight="10500" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="137">
   <si>
     <t>Metadata name</t>
   </si>
@@ -371,6 +371,9 @@
     <t>Used for our own special purpose</t>
   </si>
   <si>
+    <t>emmo:Molecule</t>
+  </si>
+  <si>
     <t>hasPart some Atom</t>
   </si>
   <si>
@@ -386,16 +389,7 @@
     <t>Molecule</t>
   </si>
   <si>
-    <t>emmo-inferred-chemistry2:Molecule</t>
-  </si>
-  <si>
-    <t>emmo-inferred-chemistry2:hasPart  some emmo-inferred-chemistry2:Atom</t>
-  </si>
-  <si>
-    <t>Test giving prefix from emmo for subclass of and relations. Will be changed to emmo: when prefix is fixed</t>
-  </si>
-  <si>
-    <t>Test giving prefix to relations. Will be changed to emmo: when prefix is fixed</t>
+    <t>emmo:hasPart  some emmo:Atom</t>
   </si>
   <si>
     <t>base_iri_root</t>
@@ -405,6 +399,48 @@
   </si>
   <si>
     <t>Local prefix for the imported ontology.</t>
+  </si>
+  <si>
+    <t>testonto</t>
+  </si>
+  <si>
+    <t>http://ontology.info/</t>
+  </si>
+  <si>
+    <t>ANewTestClass</t>
+  </si>
+  <si>
+    <t>testonto:TestClass</t>
+  </si>
+  <si>
+    <t>imported_onto/ontology.ttl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>Comment for test</t>
+  </si>
+  <si>
+    <t>Do not give base_iri_root, but leave spaces there (so it is not completely empty)</t>
+  </si>
+  <si>
+    <t>Check that prefix is set to first import (ontology.ttl)</t>
+  </si>
+  <si>
+    <t>AnotherNewTestClass</t>
+  </si>
+  <si>
+    <t>testonto:TestClass2</t>
+  </si>
+  <si>
+    <t>Test giving prefix to relations.</t>
+  </si>
+  <si>
+    <t>Test giving prefix from emmo for subclass of and relations. Prefix is set by choice in ImportedOntologies.</t>
+  </si>
+  <si>
+    <t>Check that prefix is set to subimport (ontology.ttl)</t>
   </si>
 </sst>
 </file>
@@ -510,7 +546,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -550,6 +586,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1081,8 +1120,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1097,10 +1136,10 @@
         <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="75" x14ac:dyDescent="0.25">
@@ -1108,10 +1147,13 @@
         <v>23</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>123</v>
+        <v>121</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1119,11 +1161,25 @@
         <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>115</v>
+        <v>116</v>
+      </c>
+      <c r="C3" t="s">
+        <v>128</v>
+      </c>
+      <c r="D3" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C4" s="18"/>
+      <c r="A4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
@@ -1141,10 +1197,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" topLeftCell="D12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1540,27 +1596,49 @@
         <v>112</v>
       </c>
       <c r="G25" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="I25" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="J25" t="s">
-        <v>120</v>
+        <v>135</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G26" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="I26" t="s">
         <v>119</v>
       </c>
       <c r="J26" t="s">
-        <v>121</v>
+        <v>134</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>125</v>
+      </c>
+      <c r="G27" t="s">
+        <v>126</v>
+      </c>
+      <c r="J27" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>132</v>
+      </c>
+      <c r="G28" t="s">
+        <v>133</v>
+      </c>
+      <c r="J28" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>